<commit_message>
WT32i test board updates
</commit_message>
<xml_diff>
--- a/Electrical/Test Boards/WT32i_Breakout/BOM.xlsx
+++ b/Electrical/Test Boards/WT32i_Breakout/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t>Designator:</t>
   </si>
@@ -194,6 +194,42 @@
     <t>http://www.mouser.com/ProductDetail/Panasonic/6TPF330M9L/?qs=/ha2pyFadujNMiKYkl16l5L5RqcolOyPDtMYxSzsjzC27tRQTotI4g==</t>
   </si>
   <si>
+    <t>C5,6</t>
+  </si>
+  <si>
+    <t>GRM1885C1H330FA01D</t>
+  </si>
+  <si>
+    <t>33pF/50V/C0G/+/-0.5pF, 0603</t>
+  </si>
+  <si>
+    <t>http://www.murata.com/~/media/webrenewal/support/library/catalog/products/capacitor/mlcc/c02e.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM1885C1H330FA01D/490-9720-1-ND/4934879</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Murata-Electronics/GRM1885C1H330FA01D/?qs=ECEo0ueu72kvzV2E3JDz6g==</t>
+  </si>
+  <si>
+    <t>L1,2</t>
+  </si>
+  <si>
+    <t>MLK1005S33NJT000</t>
+  </si>
+  <si>
+    <t>33nH+/-5%, 200mA, 0.9ohm, 0402</t>
+  </si>
+  <si>
+    <t>https://product.tdk.com/info/en/catalog/datasheets/inductor_commercial_high-frequency_mlk1005_en.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-corporation/MLK1005S33NJT000/445-1473-1-ND/571781</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TDK/MLK1005S33NJT000/?qs=/PzWLGNeQ%2Bg00frD1iDUEg==</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -233,16 +269,19 @@
     <t>R3,4</t>
   </si>
   <si>
-    <t>ERJ-3EKF1004V</t>
-  </si>
-  <si>
-    <t>1M/50V/0.1W/5%</t>
-  </si>
-  <si>
-    <t>0603</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1004V/?qs=sGAEpiMZZMvdGkrng054t0%2BHUCiQWsKuNf5rwThNORQ=</t>
+    <t>ERJ-3GEYJ105V</t>
+  </si>
+  <si>
+    <t>1M/50V/0.1W/5%, 0603</t>
+  </si>
+  <si>
+    <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0001+ERJ3GEYJ105V+7+WW</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-search/en/resistors/chip-resistor-surface-mount/65769?k=&amp;pkeyword=&amp;v=10&amp;FV=40025,c0002,1c0002,142c040c,fff40001,fff800e9,80002&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3GEYJ105V/?qs=66DK8nO8gJAFuT6JGu2rQw==</t>
   </si>
   <si>
     <t>P1</t>
@@ -281,16 +320,16 @@
     <t>P3</t>
   </si>
   <si>
-    <t>68000-102HLF</t>
-  </si>
-  <si>
-    <t>01X02 Male Through Hole Header</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/amphenol-fci/68000-102HLF/609-3500-ND/1493545</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-102HLF/?qs=sGAEpiMZZMs%2BGHln7q6pm44kDepmYTI8DTUYDSs9vjw=</t>
+    <t>68000-103HLF</t>
+  </si>
+  <si>
+    <t>01X03 Male Through Hole Header</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/amphenol-fci/68000-103HLF/609-3461-ND/2023309</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-103HLF/?qs=zh4O8xspOuyqPBhcuxtliw==</t>
   </si>
   <si>
     <t>ANT1</t>
@@ -428,7 +467,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -477,10 +516,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -506,10 +541,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="1:20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
@@ -1807,10 +1842,10 @@
         <v>59</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>60</v>
@@ -1827,14 +1862,16 @@
       <c r="H10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>0.1</v>
@@ -1854,14 +1891,16 @@
       <c r="H11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>0.1</v>
@@ -1872,139 +1911,194 @@
       <c r="E12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="H12" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>0.19</v>
+        <v>0.32</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="I15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>5</v>
+        <v>0.32</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13"/>
-      <c r="C17" s="6"/>
-      <c r="H17" s="0"/>
+      <c r="A17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14" t="s">
-        <v>98</v>
+      <c r="A18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="C18" s="6" t="n">
-        <f aca="false">(C2*B2)+(C3*B3)+(C4*B4)+(C5*B5)+(C6*B6)+(C7*B7)+(C8*B8)+(C9*B9)+(C10*B10)+(C11*B11)+(C12*B12)+(C13*B13)+(C14*B14)+(C15*B15)+(C16*B16)</f>
-        <v>33.61</v>
-      </c>
-      <c r="H18" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="9"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="12"/>
+      <c r="C19" s="6"/>
+      <c r="H19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <f aca="false">(C2*B2)+(C3*B3)+(C4*B4)+(C5*B5)+(C6*B6)+(C7*B7)+(C8*B8)+(C9*B9)+(C12*B12)+(C13*B13)+(C14*B14)+(C15*B15)+(C16*B16)+(C17*B17)+(C18*B18)</f>
+        <v>33.69</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://media.digikey.com/pdf/Data Sheets/BlueGiga PDFs/WT32i_DS_V1.21.pdf"/>
@@ -2033,25 +2127,33 @@
     <hyperlink ref="H9" r:id="rId24" display="http://www.mouser.com/ProductDetail/Kemet/T520D337M006ATE009/?qs=F4vAmCFCeavzfa2EBT2i1w=="/>
     <hyperlink ref="J9" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/6TPF330M9L/P16258CT-ND/4146701"/>
     <hyperlink ref="K9" r:id="rId26" display="http://www.mouser.com/ProductDetail/Panasonic/6TPF330M9L/?qs=/ha2pyFadujNMiKYkl16l5L5RqcolOyPDtMYxSzsjzC27tRQTotI4g=="/>
-    <hyperlink ref="F10" r:id="rId27" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
-    <hyperlink ref="G10" r:id="rId28" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
-    <hyperlink ref="H10" r:id="rId29" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g=="/>
-    <hyperlink ref="F11" r:id="rId30" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF8200V+7+WW"/>
-    <hyperlink ref="G11" r:id="rId31" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF8200V/P820HCT-ND/1746806"/>
-    <hyperlink ref="H11" r:id="rId32" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF8200V/?qs=/ha2pyFaduglTbPDDZSypYYGUgtAbfv2yF2HHUYX9QFp3giBobQZgg=="/>
-    <hyperlink ref="H12" r:id="rId33" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1004V/?qs=sGAEpiMZZMvdGkrng054t0%2BHUCiQWsKuNf5rwThNORQ="/>
-    <hyperlink ref="F13" r:id="rId34" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
-    <hyperlink ref="G13" r:id="rId35" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-206HLF/609-3256-ND/1878496"/>
-    <hyperlink ref="H13" r:id="rId36" display="http://www.mouser.com/ProductDetail/FCI-Amphenol/68000-206HLF/?qs=/ha2pyFaduhlIpyyGyfHK4CVidxKrihFgGI0zgkweIhxJCKanagsiA=="/>
-    <hyperlink ref="F14" r:id="rId37" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
-    <hyperlink ref="G14" r:id="rId38" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-104HLF/609-3248-ND/1878462"/>
-    <hyperlink ref="H14" r:id="rId39" display="http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-104HLF/?qs=sGAEpiMZZMs%2BGHln7q6pm24n0txessAMEGzW759vXJk="/>
-    <hyperlink ref="F15" r:id="rId40" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
-    <hyperlink ref="G15" r:id="rId41" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-102HLF/609-3500-ND/1493545"/>
-    <hyperlink ref="H15" r:id="rId42" display="http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-102HLF/?qs=sGAEpiMZZMs%2BGHln7q6pm44kDepmYTI8DTUYDSs9vjw="/>
-    <hyperlink ref="F16" r:id="rId43" display="http://www.lsr.com/downloads/products/330-0150.pdf"/>
-    <hyperlink ref="G16" r:id="rId44" display="https://www.digikey.com/product-detail/en/lsr/001-0015/001-0015-ND/4732759"/>
-    <hyperlink ref="H16" r:id="rId45" display="http://www.mouser.com/ProductDetail/LS-Research/001-0015/?qs=sGAEpiMZZMuBTKBKvsBmlP%2BmDojcpAG/Vyhv39d/eWhHn2QU78Oagg=="/>
+    <hyperlink ref="F10" r:id="rId27" display="http://www.murata.com/~/media/webrenewal/support/library/catalog/products/capacitor/mlcc/c02e.pdf"/>
+    <hyperlink ref="G10" r:id="rId28" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM1885C1H330FA01D/490-9720-1-ND/4934879"/>
+    <hyperlink ref="H10" r:id="rId29" display="http://www.mouser.com/ProductDetail/Murata-Electronics/GRM1885C1H330FA01D/?qs=ECEo0ueu72kvzV2E3JDz6g=="/>
+    <hyperlink ref="F11" r:id="rId30" display="https://product.tdk.com/info/en/catalog/datasheets/inductor_commercial_high-frequency_mlk1005_en.pdf"/>
+    <hyperlink ref="G11" r:id="rId31" display="https://www.digikey.com/product-detail/en/tdk-corporation/MLK1005S33NJT000/445-1473-1-ND/571781"/>
+    <hyperlink ref="H11" r:id="rId32" display="http://www.mouser.com/ProductDetail/TDK/MLK1005S33NJT000/?qs=/PzWLGNeQ%2Bg00frD1iDUEg=="/>
+    <hyperlink ref="F12" r:id="rId33" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
+    <hyperlink ref="G12" r:id="rId34" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
+    <hyperlink ref="H12" r:id="rId35" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g=="/>
+    <hyperlink ref="F13" r:id="rId36" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF8200V+7+WW"/>
+    <hyperlink ref="G13" r:id="rId37" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF8200V/P820HCT-ND/1746806"/>
+    <hyperlink ref="H13" r:id="rId38" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF8200V/?qs=/ha2pyFaduglTbPDDZSypYYGUgtAbfv2yF2HHUYX9QFp3giBobQZgg=="/>
+    <hyperlink ref="F14" r:id="rId39" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0001+ERJ3GEYJ105V+7+WW"/>
+    <hyperlink ref="G14" r:id="rId40" display="https://www.digikey.com/product-search/en/resistors/chip-resistor-surface-mount/65769?k=&amp;pkeyword=&amp;v=10&amp;FV=40025,c0002,1c0002,142c040c,fff40001,fff800e9,80002&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25"/>
+    <hyperlink ref="H14" r:id="rId41" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3GEYJ105V/?qs=66DK8nO8gJAFuT6JGu2rQw=="/>
+    <hyperlink ref="F15" r:id="rId42" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
+    <hyperlink ref="G15" r:id="rId43" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-206HLF/609-3256-ND/1878496"/>
+    <hyperlink ref="H15" r:id="rId44" display="http://www.mouser.com/ProductDetail/FCI-Amphenol/68000-206HLF/?qs=/ha2pyFaduhlIpyyGyfHK4CVidxKrihFgGI0zgkweIhxJCKanagsiA=="/>
+    <hyperlink ref="F16" r:id="rId45" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
+    <hyperlink ref="G16" r:id="rId46" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-104HLF/609-3248-ND/1878462"/>
+    <hyperlink ref="H16" r:id="rId47" display="http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-104HLF/?qs=sGAEpiMZZMs%2BGHln7q6pm24n0txessAMEGzW759vXJk="/>
+    <hyperlink ref="F17" r:id="rId48" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
+    <hyperlink ref="G17" r:id="rId49" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-103HLF/609-3461-ND/2023309"/>
+    <hyperlink ref="H17" r:id="rId50" display="http://www.mouser.com/ProductDetail/Amphenol-FCI/68000-103HLF/?qs=zh4O8xspOuyqPBhcuxtliw=="/>
+    <hyperlink ref="F18" r:id="rId51" display="http://www.lsr.com/downloads/products/330-0150.pdf"/>
+    <hyperlink ref="G18" r:id="rId52" display="https://www.digikey.com/product-detail/en/lsr/001-0015/001-0015-ND/4732759"/>
+    <hyperlink ref="H18" r:id="rId53" display="http://www.mouser.com/ProductDetail/LS-Research/001-0015/?qs=sGAEpiMZZMuBTKBKvsBmlP%2BmDojcpAG/Vyhv39d/eWhHn2QU78Oagg=="/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>